<commit_message>
Changes saved upto 28-08-2023
</commit_message>
<xml_diff>
--- a/RR/excel/Appriciate_Flow.xlsx
+++ b/RR/excel/Appriciate_Flow.xlsx
@@ -8,15 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\choug\git\RR_Web\RR\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E230DD0-34F8-4558-A061-A831574ED7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94E9D86-9825-4D96-8D76-B0AB6553713E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="C1227" sheetId="1" r:id="rId1"/>
-    <sheet name="C900" sheetId="2" r:id="rId2"/>
+    <sheet name="C900" sheetId="2" r:id="rId1"/>
+    <sheet name="C466" sheetId="10" r:id="rId2"/>
+    <sheet name="C1214" sheetId="4" r:id="rId3"/>
+    <sheet name="C1227" sheetId="5" r:id="rId4"/>
+    <sheet name="C1270" sheetId="6" r:id="rId5"/>
+    <sheet name="C943" sheetId="7" r:id="rId6"/>
+    <sheet name="C1083" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +36,7 @@
     <author>Dheeraj Chougule</author>
   </authors>
   <commentList>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{3695F861-CA65-4025-B1AA-E8B2501C422D}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{FBC9A22B-C228-4C51-A9B5-AE6170461400}">
       <text>
         <r>
           <rPr>
@@ -55,7 +60,127 @@
     <author>Dheeraj Chougule</author>
   </authors>
   <commentList>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{FBC9A22B-C228-4C51-A9B5-AE6170461400}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{D4BD7996-1FE7-4277-A182-2287B9851769}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>if team is there then need to add mail according to count</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dheeraj Chougule</author>
+  </authors>
+  <commentList>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{A9BF3E29-11D6-4B6D-AAF5-7AC07B8E93CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>if team is there then need to add mail according to count</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dheeraj Chougule</author>
+  </authors>
+  <commentList>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{9C06724C-AB9B-48EC-99C6-1EB05475350A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>if team is there then need to add mail according to count</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dheeraj Chougule</author>
+  </authors>
+  <commentList>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{BDDF7AB5-86D2-455A-8A79-A874112D8D3C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>if team is there then need to add mail according to count</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dheeraj Chougule</author>
+  </authors>
+  <commentList>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{748E4592-464C-4918-A856-8FB9C715417D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>if team is there then need to add mail according to count</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dheeraj Chougule</author>
+  </authors>
+  <commentList>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{09C216B5-72D1-43D7-9345-5E1FDE4540DA}">
       <text>
         <r>
           <rPr>
@@ -74,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="84">
   <si>
     <t>Appriciate By</t>
   </si>
@@ -118,9 +243,6 @@
     <t>known</t>
   </si>
   <si>
-    <t>any</t>
-  </si>
-  <si>
     <t>single</t>
   </si>
   <si>
@@ -145,9 +267,6 @@
     <t>testdemo</t>
   </si>
   <si>
-    <t>employeeactest1@yopmail.com</t>
-  </si>
-  <si>
     <t>manageractest1@yopmail.com</t>
   </si>
   <si>
@@ -158,13 +277,187 @@
   </si>
   <si>
     <t>employeeactest3@yopmail.com</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>projectmanager.satven@outlook.com</t>
+  </si>
+  <si>
+    <t>Advantage!1270</t>
+  </si>
+  <si>
+    <t>Nominee1.satven@outlook.com</t>
+  </si>
+  <si>
+    <t>Error Validation message</t>
+  </si>
+  <si>
+    <t>Mail wrong and submit</t>
+  </si>
+  <si>
+    <t>Mail not given and submit</t>
+  </si>
+  <si>
+    <t>Add at least one recipient.</t>
+  </si>
+  <si>
+    <t>Please enter valid email or name.</t>
+  </si>
+  <si>
+    <t>Same mail given 2 times</t>
+  </si>
+  <si>
+    <t>Please select a different user.</t>
+  </si>
+  <si>
+    <t>employeeacte@yopmail.com</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Cases</t>
+  </si>
+  <si>
+    <t>Not selecting award and submit</t>
+  </si>
+  <si>
+    <t>Mandetory</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Mandetory / Non-Mandetory</t>
+  </si>
+  <si>
+    <t>No message and Submit</t>
+  </si>
+  <si>
+    <t>Please provide the message.</t>
+  </si>
+  <si>
+    <t>card Specific (Available)</t>
+  </si>
+  <si>
+    <t>card Specific (Required)</t>
+  </si>
+  <si>
+    <t>card Specific (Name)</t>
+  </si>
+  <si>
+    <t>Card Needed</t>
+  </si>
+  <si>
+    <t>manager1.sentiss@yopmail.com</t>
+  </si>
+  <si>
+    <t>Advantage!1214</t>
+  </si>
+  <si>
+    <t>employee1.sentiss@yopmail.com</t>
+  </si>
+  <si>
+    <t>Add an award.</t>
+  </si>
+  <si>
+    <t>manager1.ac@yopmail.com</t>
+  </si>
+  <si>
+    <t>employee1.ac@yopmail.com</t>
+  </si>
+  <si>
+    <t>employee2.ac@yopmail.com</t>
+  </si>
+  <si>
+    <t>Advantage!0198</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>nominatorsteel@ac.in</t>
+  </si>
+  <si>
+    <t>advantage!943</t>
+  </si>
+  <si>
+    <t>buheadsteel@ac.in</t>
+  </si>
+  <si>
+    <t>Satven</t>
+  </si>
+  <si>
+    <t>employeeactest4@yopmail.com</t>
+  </si>
+  <si>
+    <t>manager1.tf@yopmail.com</t>
+  </si>
+  <si>
+    <t>employee1.tf@yopmail.com</t>
+  </si>
+  <si>
+    <t>Advantage!1084</t>
+  </si>
+  <si>
+    <t>NewsFeed Testing</t>
+  </si>
+  <si>
+    <t>Like (Available)</t>
+  </si>
+  <si>
+    <t>Comment (Availble)</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Like (Required)</t>
+  </si>
+  <si>
+    <t>Comment (Required)</t>
+  </si>
+  <si>
+    <t>Nicely Done</t>
+  </si>
+  <si>
+    <t>manageractest2@yopmail.com</t>
+  </si>
+  <si>
+    <t>Multiple buzz Created ??</t>
+  </si>
+  <si>
+    <t>employee5.ac@yopmail.com</t>
+  </si>
+  <si>
+    <t>employee3.ac@yopmail.com</t>
+  </si>
+  <si>
+    <t>manager16@rewards-demo.com</t>
+  </si>
+  <si>
+    <t>ZZXDI4VW</t>
+  </si>
+  <si>
+    <t>kabir@yopmail.com</t>
+  </si>
+  <si>
+    <t>manager17@rewards-demo.com</t>
+  </si>
+  <si>
+    <t>employee1@rewards-demo.com</t>
+  </si>
+  <si>
+    <t>employee2@rewards-demo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +484,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -223,12 +523,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -509,20 +813,686 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5715155E-D895-4370-B1A9-378741347274}">
+  <dimension ref="A3:I66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{47DE3FE4-F463-4AB2-ABF1-8C6FC3BE9BA8}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{4F83EBF1-044A-4508-BCB9-8D89517ABF72}"/>
+    <hyperlink ref="C52" r:id="rId3" xr:uid="{8723B52D-DB5F-4456-B419-F6E169BED2D0}"/>
+    <hyperlink ref="D11" r:id="rId4" xr:uid="{D63146EF-4505-478D-BF64-CBF7D1C68569}"/>
+    <hyperlink ref="E11" r:id="rId5" xr:uid="{B0B674D2-7470-4A17-99D0-3AF3DA1347D2}"/>
+    <hyperlink ref="C30" r:id="rId6" xr:uid="{3AEE9EA8-375A-4C2C-95D0-E1CEBECC9267}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C353D1-B0D2-4862-AB53-0799460CD224}">
+  <dimension ref="A3:I66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{A6CA4FFC-409F-4606-A31C-944634A51C40}"/>
+    <hyperlink ref="C52" r:id="rId2" xr:uid="{42C7859C-AE64-435F-B93B-369BA83A29D7}"/>
+    <hyperlink ref="E11" r:id="rId3" xr:uid="{10B33063-5355-449F-93A1-972067C3E1E9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1904D5E4-442E-4BF4-A39A-8D603AE31D02}">
+  <dimension ref="A3:F66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -538,10 +1508,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -566,7 +1536,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -580,6 +1550,12 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -599,7 +1575,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -609,96 +1585,233 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
       <c r="C29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>21</v>
-      </c>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>22</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{D788E2E1-7C5A-432E-A3FC-10B1D72EA6A6}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{53C84025-42C8-4A66-BD3B-C97EE9B5054C}"/>
-    <hyperlink ref="C30" r:id="rId3" xr:uid="{EA286428-91FD-4FCE-9945-29569AD5D0E1}"/>
+    <hyperlink ref="C52" r:id="rId1" xr:uid="{E8410BE1-72E6-4B49-BB6C-E6E714101565}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5715155E-D895-4370-B1A9-378741347274}">
-  <dimension ref="A3:E31"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89CAEB5-4F1C-4B6A-A4C1-C7B6352E777E}">
+  <dimension ref="A3:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -714,10 +1827,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,7 +1841,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -742,7 +1855,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -756,6 +1869,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -775,87 +1896,1203 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{2B3985A1-2482-4253-9AD3-AF2AD120032D}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{DFC35F61-603F-4F0A-8821-B5FDDEA55313}"/>
+    <hyperlink ref="C30" r:id="rId3" xr:uid="{635C71BF-90BC-488F-97A6-D838A2AF2B3A}"/>
+    <hyperlink ref="C52" r:id="rId4" xr:uid="{AAE3206D-281E-433C-88D3-31DEE0CF5F9D}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{4B37A0C8-9902-4B3A-8C48-207A62C2C440}"/>
+    <hyperlink ref="E11" r:id="rId6" xr:uid="{AB02DB5B-9CF2-4711-B7D2-2BBEB97F4072}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01DDC2E-4DD9-4530-B52D-604A1B3036DF}">
+  <dimension ref="A1:F66"/>
+  <sheetViews>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C1" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>21</v>
-      </c>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{47DE3FE4-F463-4AB2-ABF1-8C6FC3BE9BA8}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{4F83EBF1-044A-4508-BCB9-8D89517ABF72}"/>
-    <hyperlink ref="C30" r:id="rId3" xr:uid="{78970880-1D10-4893-9D69-FDF10E84A11A}"/>
+    <hyperlink ref="C52" r:id="rId1" xr:uid="{515FEB38-EE19-44E2-B45D-E3DDAF284025}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139DD397-4634-4FB8-8587-B601CEB59A8E}">
+  <dimension ref="A3:F66"/>
+  <sheetViews>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{6FADE9A6-F4AE-4526-AB84-08443FE54E83}"/>
+    <hyperlink ref="C30" r:id="rId2" xr:uid="{C95B1009-3F41-446C-A97E-6DC19A2A2D9D}"/>
+    <hyperlink ref="C52" r:id="rId3" xr:uid="{06276366-17F9-4D02-B30E-7BF065BC7B1D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF140F85-C10E-4600-8D6D-D3607B55159B}">
+  <dimension ref="A3:F66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C30" r:id="rId1" xr:uid="{688DD04C-2ED4-437E-B80B-D0F57FC7FD52}"/>
+    <hyperlink ref="C52" r:id="rId2" xr:uid="{2F75E27C-219D-409E-BE3A-5717289E23AF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new commit on 6-1-24
</commit_message>
<xml_diff>
--- a/RR/excel/Appriciate_Flow.xlsx
+++ b/RR/excel/Appriciate_Flow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\choug\git\RR_Web\RR\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86607F49-4A7C-4E20-8F58-FE9B488414BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE8B255-A480-4DD5-BD8B-BC55A039513C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C900" sheetId="2" r:id="rId1"/>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="153">
   <si>
     <t>Appriciate By</t>
   </si>
@@ -604,12 +604,6 @@
     <t>manager16@rewards-demo.com</t>
   </si>
   <si>
-    <t>ZZXDI4VW</t>
-  </si>
-  <si>
-    <t>kabir@yopmail.com</t>
-  </si>
-  <si>
     <t>manager17@rewards-demo.com</t>
   </si>
   <si>
@@ -806,13 +800,46 @@
   </si>
   <si>
     <t>tl1.ainindia@yopmail.com</t>
+  </si>
+  <si>
+    <t>014kx4gnxx</t>
+  </si>
+  <si>
+    <t>lukecooper@yopmail.com</t>
+  </si>
+  <si>
+    <t>Luke Cooper</t>
+  </si>
+  <si>
+    <t>MY PROFILE</t>
+  </si>
+  <si>
+    <t>Wallet Name</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Wellness</t>
+  </si>
+  <si>
+    <t>Wallet Count</t>
+  </si>
+  <si>
+    <t>Appreciated list</t>
+  </si>
+  <si>
+    <t>Awarded list</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,6 +905,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -918,7 +953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -946,6 +981,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1230,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5715155E-D895-4370-B1A9-378741347274}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,12 +1286,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I2" s="16"/>
     </row>
@@ -1265,9 +1303,11 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1371,7 +1411,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1430,7 +1470,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1444,7 +1484,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1462,7 +1502,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1537,12 +1577,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -1636,12 +1676,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1652,7 +1692,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>23</v>
@@ -1663,10 +1703,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3"/>
@@ -1735,13 +1775,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1754,7 +1794,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,7 +1857,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1831,7 +1871,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1851,7 +1891,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1922,12 +1962,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>56</v>
@@ -2021,12 +2061,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2037,7 +2077,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>23</v>
@@ -2048,10 +2088,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3"/>
@@ -2118,10 +2158,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -2135,7 +2175,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2194,7 +2234,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,7 +2248,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,7 +2268,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2299,12 +2339,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -2398,12 +2438,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2414,7 +2454,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="10"/>
@@ -2425,10 +2465,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3"/>
@@ -2497,10 +2537,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -2514,7 +2554,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2573,7 +2613,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2587,7 +2627,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2609,7 +2649,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2680,12 +2720,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -2779,12 +2819,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2795,7 +2835,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="10"/>
@@ -2806,10 +2846,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3"/>
@@ -2878,13 +2918,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2897,7 +2937,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2956,7 +2996,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2970,7 +3010,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2992,7 +3032,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3063,12 +3103,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -3125,7 +3165,7 @@
         <v>43</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3144,8 +3184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6E741F-8C66-4FFE-B62A-99CC18C85D65}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3162,12 +3202,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I2" s="16"/>
     </row>
@@ -3179,7 +3219,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -3188,10 +3228,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -3259,13 +3299,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3273,13 +3313,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3287,7 +3327,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3346,7 +3386,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3360,7 +3400,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3378,7 +3418,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3453,12 +3493,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -3532,10 +3572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C353D1-B0D2-4862-AB53-0799460CD224}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3552,12 +3592,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3568,7 +3608,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -3580,7 +3620,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3647,13 +3687,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3664,9 +3704,14 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3716,7 +3761,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>47</v>
@@ -3725,7 +3770,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3739,7 +3784,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3757,7 +3802,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3776,7 +3821,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3830,12 +3875,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -3884,7 +3929,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>43</v>
       </c>
@@ -3892,7 +3937,58 @@
         <v>44</v>
       </c>
     </row>
+    <row r="71" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B79" t="s">
+        <v>147</v>
+      </c>
+      <c r="C79" t="s">
+        <v>148</v>
+      </c>
+      <c r="D79" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B82" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B83" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A76:E76"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" xr:uid="{A6CA4FFC-409F-4606-A31C-944634A51C40}"/>
     <hyperlink ref="C52" r:id="rId2" xr:uid="{42C7859C-AE64-435F-B93B-369BA83A29D7}"/>
@@ -3925,12 +4021,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3941,7 +4037,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -4034,7 +4130,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4091,7 +4187,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4105,7 +4201,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4125,7 +4221,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4200,12 +4296,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -4280,7 +4376,7 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4296,12 +4392,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4312,7 +4408,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -4390,13 +4486,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4409,7 +4505,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4472,7 +4568,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4486,7 +4582,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4504,7 +4600,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4577,12 +4673,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -4684,7 +4780,7 @@
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4695,7 +4791,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -4773,10 +4869,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -4792,7 +4888,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4847,7 +4943,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4861,7 +4957,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4879,7 +4975,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4952,12 +5048,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>23</v>
@@ -5050,12 +5146,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5066,7 +5162,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -5159,7 +5255,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5218,7 +5314,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -5232,7 +5328,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5250,7 +5346,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -5282,7 +5378,7 @@
     </row>
     <row r="35" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5325,12 +5421,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -5423,12 +5519,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5439,7 +5535,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -5520,7 +5616,7 @@
         <v>63</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -5538,7 +5634,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5597,7 +5693,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -5611,7 +5707,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5629,7 +5725,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -5704,12 +5800,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -5803,12 +5899,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5819,7 +5915,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -5828,10 +5924,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5898,13 +5994,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -5917,7 +6013,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5976,7 +6072,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -5990,7 +6086,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -6008,7 +6104,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -6027,7 +6123,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -6081,12 +6177,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -6180,12 +6276,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -6196,7 +6292,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -6205,10 +6301,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6275,10 +6371,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -6292,7 +6388,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -6351,7 +6447,7 @@
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -6365,7 +6461,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -6387,7 +6483,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -6406,7 +6502,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -6460,12 +6556,12 @@
     </row>
     <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>

</xml_diff>